<commit_message>
Working simple optimisation just for parameters without any covariates.
</commit_message>
<xml_diff>
--- a/Manual optimisation calculation.xlsx
+++ b/Manual optimisation calculation.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aydin\OneDrive\Documents\Research\multivariate-joint-regression-simulation-study\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8446EF30-9DEC-4E2E-B95D-658C22E11DFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AA6392D-6AE5-4B9C-BE67-672E4CCCCEA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="27288" windowHeight="17544" xr2:uid="{49D03924-E1C7-4E8A-A057-1B73C7C85AF8}"/>
+    <workbookView xWindow="-9684" yWindow="-26028" windowWidth="46296" windowHeight="26136" activeTab="1" xr2:uid="{49D03924-E1C7-4E8A-A057-1B73C7C85AF8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Copula" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="solver_adj" localSheetId="0" hidden="1">Sheet1!$L$11</definedName>
@@ -65,7 +66,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="86">
   <si>
     <t>subject</t>
   </si>
@@ -253,18 +254,6 @@
     <t>DLDTH</t>
   </si>
   <si>
-    <t>Sum</t>
-  </si>
-  <si>
-    <t>Average</t>
-  </si>
-  <si>
-    <t>Running Total</t>
-  </si>
-  <si>
-    <t>Count</t>
-  </si>
-  <si>
     <t>log(COPULA_D)</t>
   </si>
   <si>
@@ -284,6 +273,57 @@
   </si>
   <si>
     <t>OLD_PAR</t>
+  </si>
+  <si>
+    <t>mu</t>
+  </si>
+  <si>
+    <t>dldm</t>
+  </si>
+  <si>
+    <t>num_dlcopdpar_ordered</t>
+  </si>
+  <si>
+    <t>num_dlcopdpar_nolog_ordered</t>
+  </si>
+  <si>
+    <t>MARGIN</t>
+  </si>
+  <si>
+    <t>COPULA</t>
+  </si>
+  <si>
+    <t>dcdu1</t>
+  </si>
+  <si>
+    <t>dcdu2</t>
+  </si>
+  <si>
+    <t>x_it</t>
+  </si>
+  <si>
+    <t>f(x_it)</t>
+  </si>
+  <si>
+    <t>F(x_it)</t>
+  </si>
+  <si>
+    <t>mu.time mu.as.factor(gender)1</t>
+  </si>
+  <si>
+    <t>1.002597              1.348431</t>
+  </si>
+  <si>
+    <t>c(F(xit),F(xi(t+1))</t>
+  </si>
+  <si>
+    <t>FOR TIME = 2</t>
+  </si>
+  <si>
+    <t>dc_tplus_dut</t>
+  </si>
+  <si>
+    <t>du_t_dmu</t>
   </si>
 </sst>
 </file>
@@ -292,9 +332,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="4">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="176" formatCode="_-* #,##0.0000_-;\-* #,##0.0000_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="182" formatCode="0.0000"/>
-    <numFmt numFmtId="183" formatCode="0.000"/>
+    <numFmt numFmtId="164" formatCode="_-* #,##0.0000_-;\-* #,##0.0000_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="165" formatCode="0.0000"/>
+    <numFmt numFmtId="166" formatCode="0.000"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -348,17 +388,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="182" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="183" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -696,8 +737,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE2333A5-6A58-41A7-B7F8-53FF6BB309B9}">
   <dimension ref="A7:BI73"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q25" sqref="Q25"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L17" sqref="L17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -866,7 +907,7 @@
         <v>2.8896449255633172E-7</v>
       </c>
       <c r="V11" s="5">
-        <f>(1/R11)*EXP(-1/R11*D11)</f>
+        <f t="shared" ref="V11:V25" si="0">(1/R11)*EXP(-1/R11*D11)</f>
         <v>5.5118753807019884E-3</v>
       </c>
       <c r="W11">
@@ -911,47 +952,47 @@
         <v>0</v>
       </c>
       <c r="N12">
-        <f t="shared" ref="N12:N25" si="0">$I$11+$J$11*C12+$K$11*G12</f>
+        <f t="shared" ref="N12:N25" si="1">$I$11+$J$11*C12+$K$11*G12</f>
         <v>5.6222642999999994</v>
       </c>
       <c r="O12">
         <v>5.6222640000000004</v>
       </c>
       <c r="P12" s="1">
-        <f t="shared" ref="P12:P25" si="1">O12/N12-1</f>
+        <f t="shared" ref="P12:P25" si="2">O12/N12-1</f>
         <v>-5.3359284324372425E-8</v>
       </c>
       <c r="R12">
-        <f t="shared" ref="R12:R25" si="2">EXP(N12)</f>
+        <f t="shared" ref="R12:R25" si="3">EXP(N12)</f>
         <v>276.51478734930225</v>
       </c>
       <c r="S12">
         <v>276.51479999999998</v>
       </c>
       <c r="T12" s="1">
-        <f t="shared" ref="T12:T25" si="3">S12/R12-1</f>
+        <f t="shared" ref="T12:T25" si="4">S12/R12-1</f>
         <v>4.5750528698818016E-8</v>
       </c>
       <c r="V12" s="5">
-        <f>(1/R12)*EXP(-1/R12*D12)</f>
+        <f t="shared" si="0"/>
         <v>1.203878284634278E-3</v>
       </c>
       <c r="W12">
         <v>1.2038783100000001E-3</v>
       </c>
       <c r="X12" s="1">
-        <f t="shared" ref="X12:X25" si="4">W12/V12-1</f>
+        <f t="shared" ref="X12:X25" si="5">W12/V12-1</f>
         <v>2.1070005518097901E-8</v>
       </c>
       <c r="Z12" s="4">
-        <f t="shared" ref="Z12:Z25" si="5">1-EXP(-(1/R12)*D12)</f>
+        <f t="shared" ref="Z12:Z25" si="6">1-EXP(-(1/R12)*D12)</f>
         <v>0.66710985212990992</v>
       </c>
       <c r="AA12" s="7">
         <v>0.66710979999999998</v>
       </c>
       <c r="AB12" s="1">
-        <f t="shared" ref="AB12:AB25" si="6">AA12/Z12-1</f>
+        <f t="shared" ref="AB12:AB25" si="7">AA12/Z12-1</f>
         <v>-7.8142917248058552E-8</v>
       </c>
     </row>
@@ -978,47 +1019,47 @@
         <v>0</v>
       </c>
       <c r="N13">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>6.6248613000000001</v>
       </c>
       <c r="O13">
         <v>6.6248610000000001</v>
       </c>
       <c r="P13" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-4.5283966909615003E-8</v>
       </c>
       <c r="R13">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>753.59968102970879</v>
       </c>
       <c r="S13">
         <v>753.59969999999998</v>
       </c>
       <c r="T13" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2.5172902429204669E-8</v>
       </c>
       <c r="V13" s="5">
-        <f>(1/R13)*EXP(-1/R13*D13)</f>
+        <f t="shared" si="0"/>
         <v>7.6371461645548288E-4</v>
       </c>
       <c r="W13">
         <v>7.6371459E-4</v>
       </c>
       <c r="X13" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>-3.4640534996022154E-8</v>
       </c>
       <c r="Z13" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0.42446490864142172</v>
       </c>
       <c r="AA13" s="7">
         <v>0.42446489999999998</v>
       </c>
       <c r="AB13" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>-2.0358389085650686E-8</v>
       </c>
     </row>
@@ -1045,47 +1086,47 @@
         <v>1</v>
       </c>
       <c r="N14">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>5.9680980999999997</v>
       </c>
       <c r="O14">
         <v>5.9680980000000003</v>
       </c>
       <c r="P14" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-1.6755756671038569E-8</v>
       </c>
       <c r="R14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>390.7617737477799</v>
       </c>
       <c r="S14">
         <v>390.76179999999999</v>
       </c>
       <c r="T14" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>6.7182160279344316E-8</v>
       </c>
       <c r="V14" s="5">
-        <f>(1/R14)*EXP(-1/R14*D14)</f>
+        <f t="shared" si="0"/>
         <v>7.6184731726219087E-4</v>
       </c>
       <c r="W14">
         <v>7.6184731000000002E-4</v>
       </c>
       <c r="X14" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>-9.5323441362538119E-9</v>
       </c>
       <c r="Z14" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0.70229919098163873</v>
       </c>
       <c r="AA14" s="7">
         <v>0.70229920000000001</v>
       </c>
       <c r="AB14" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1.284119566236086E-8</v>
       </c>
     </row>
@@ -1112,47 +1153,47 @@
         <v>1</v>
       </c>
       <c r="N15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>6.9706950999999995</v>
       </c>
       <c r="O15">
         <v>6.9706950000000001</v>
       </c>
       <c r="P15" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-1.4345771570667409E-8</v>
       </c>
       <c r="R15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1064.9627489286352</v>
       </c>
       <c r="S15">
         <v>1064.9628</v>
       </c>
       <c r="T15" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>4.7956010496008616E-8</v>
       </c>
       <c r="V15" s="5">
-        <f>(1/R15)*EXP(-1/R15*D15)</f>
+        <f t="shared" si="0"/>
         <v>2.7729502864469945E-4</v>
       </c>
       <c r="W15">
         <v>2.7729502999999998E-4</v>
       </c>
       <c r="X15" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>4.8875758995592378E-9</v>
       </c>
       <c r="Z15" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0.70469112403029621</v>
       </c>
       <c r="AA15" s="7">
         <v>0.70469110000000001</v>
       </c>
       <c r="AB15" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>-3.4100466672626339E-8</v>
       </c>
     </row>
@@ -1179,47 +1220,47 @@
         <v>1</v>
       </c>
       <c r="N16">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>7.9732921000000001</v>
       </c>
       <c r="O16">
         <v>7.9732919999999998</v>
       </c>
       <c r="P16" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-1.2541870875182326E-8</v>
       </c>
       <c r="R16">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2902.3966334477723</v>
       </c>
       <c r="S16">
         <v>2902.3968</v>
       </c>
       <c r="T16" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>5.7384378804314906E-8</v>
       </c>
       <c r="V16" s="5">
-        <f>(1/R16)*EXP(-1/R16*D16)</f>
+        <f t="shared" si="0"/>
         <v>2.2202445851161176E-4</v>
       </c>
       <c r="W16">
         <v>2.2202444999999999E-4</v>
       </c>
       <c r="X16" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>-3.8336369967417738E-8</v>
       </c>
       <c r="Z16" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0.3555969590728334</v>
       </c>
       <c r="AA16" s="7">
         <v>0.35559689999999999</v>
       </c>
       <c r="AB16" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>-1.6612299935658825E-7</v>
       </c>
     </row>
@@ -1246,47 +1287,47 @@
         <v>0</v>
       </c>
       <c r="N17">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4.6196672999999997</v>
       </c>
       <c r="O17">
         <v>4.6196669999999997</v>
       </c>
       <c r="P17" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-6.4939741473146739E-8</v>
       </c>
       <c r="R17">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>101.46027068158438</v>
       </c>
       <c r="S17">
         <v>101.4603</v>
       </c>
       <c r="T17" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2.8896449255633172E-7</v>
       </c>
       <c r="V17" s="5">
-        <f>(1/R17)*EXP(-1/R17*D17)</f>
+        <f t="shared" si="0"/>
         <v>1.3838091009871949E-3</v>
       </c>
       <c r="W17">
         <v>1.38380914E-3</v>
       </c>
       <c r="X17" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>2.8192331580356722E-8</v>
       </c>
       <c r="Z17" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0.85959835404219931</v>
       </c>
       <c r="AA17" s="7">
         <v>0.85959830000000004</v>
       </c>
       <c r="AB17" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>-6.2869128347742276E-8</v>
       </c>
     </row>
@@ -1313,47 +1354,47 @@
         <v>0</v>
       </c>
       <c r="N18">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>5.6222642999999994</v>
       </c>
       <c r="O18">
         <v>5.6222640000000004</v>
       </c>
       <c r="P18" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-5.3359284324372425E-8</v>
       </c>
       <c r="R18">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>276.51478734930225</v>
       </c>
       <c r="S18">
         <v>276.51479999999998</v>
       </c>
       <c r="T18" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>4.5750528698818016E-8</v>
       </c>
       <c r="V18" s="5">
-        <f>(1/R18)*EXP(-1/R18*D18)</f>
+        <f t="shared" si="0"/>
         <v>4.4745097750873683E-4</v>
       </c>
       <c r="W18">
         <v>4.4745099000000001E-4</v>
       </c>
       <c r="X18" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>2.7916495559665577E-8</v>
       </c>
       <c r="Z18" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0.87627318810493415</v>
       </c>
       <c r="AA18" s="7">
         <v>0.87627319999999997</v>
       </c>
       <c r="AB18" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1.3574608992428239E-8</v>
       </c>
     </row>
@@ -1380,47 +1421,47 @@
         <v>0</v>
       </c>
       <c r="N19">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>6.6248613000000001</v>
       </c>
       <c r="O19">
         <v>6.6248610000000001</v>
       </c>
       <c r="P19" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-4.5283966909615003E-8</v>
       </c>
       <c r="R19">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>753.59968102970879</v>
       </c>
       <c r="S19">
         <v>753.59969999999998</v>
       </c>
       <c r="T19" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2.5172902429204669E-8</v>
       </c>
       <c r="V19" s="5">
-        <f>(1/R19)*EXP(-1/R19*D19)</f>
+        <f t="shared" si="0"/>
         <v>4.2880977384323628E-4</v>
       </c>
       <c r="W19">
         <v>4.2880978000000002E-4</v>
       </c>
       <c r="X19" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1.4357797173403242E-8</v>
       </c>
       <c r="Z19" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0.67684909120931558</v>
       </c>
       <c r="AA19" s="7">
         <v>0.67684909999999998</v>
       </c>
       <c r="AB19" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1.2987657838081645E-8</v>
       </c>
     </row>
@@ -1447,47 +1488,47 @@
         <v>0</v>
       </c>
       <c r="N20">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4.6196672999999997</v>
       </c>
       <c r="O20">
         <v>4.6196669999999997</v>
       </c>
       <c r="P20" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-6.4939741473146739E-8</v>
       </c>
       <c r="R20">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>101.46027068158438</v>
       </c>
       <c r="S20">
         <v>101.4603</v>
       </c>
       <c r="T20" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2.8896449255633172E-7</v>
       </c>
       <c r="V20" s="5">
-        <f>(1/R20)*EXP(-1/R20*D20)</f>
+        <f t="shared" si="0"/>
         <v>6.3935206104983218E-3</v>
       </c>
       <c r="W20">
         <v>6.3935204099999999E-3</v>
       </c>
       <c r="X20" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>-3.1359611463166459E-8</v>
       </c>
       <c r="Z20" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0.35131166825055171</v>
       </c>
       <c r="AA20" s="7">
         <v>0.3513117</v>
       </c>
       <c r="AB20" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>9.0374021599615162E-8</v>
       </c>
     </row>
@@ -1514,47 +1555,47 @@
         <v>0</v>
       </c>
       <c r="N21">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>5.6222642999999994</v>
       </c>
       <c r="O21">
         <v>5.6222640000000004</v>
       </c>
       <c r="P21" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-5.3359284324372425E-8</v>
       </c>
       <c r="R21">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>276.51478734930225</v>
       </c>
       <c r="S21">
         <v>276.51479999999998</v>
       </c>
       <c r="T21" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>4.5750528698818016E-8</v>
       </c>
       <c r="V21" s="5">
-        <f>(1/R21)*EXP(-1/R21*D21)</f>
+        <f t="shared" si="0"/>
         <v>2.4183426392456373E-3</v>
       </c>
       <c r="W21">
         <v>2.4183425699999999E-3</v>
       </c>
       <c r="X21" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>-2.8633509674413915E-8</v>
       </c>
       <c r="Z21" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0.33129249937124228</v>
       </c>
       <c r="AA21" s="7">
         <v>0.33129249999999999</v>
       </c>
       <c r="AB21" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1.8978929539059664E-9</v>
       </c>
     </row>
@@ -1581,47 +1622,47 @@
         <v>0</v>
       </c>
       <c r="N22">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>6.6248613000000001</v>
       </c>
       <c r="O22">
         <v>6.6248610000000001</v>
       </c>
       <c r="P22" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-4.5283966909615003E-8</v>
       </c>
       <c r="R22">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>753.59968102970879</v>
       </c>
       <c r="S22">
         <v>753.59969999999998</v>
       </c>
       <c r="T22" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2.5172902429204669E-8</v>
       </c>
       <c r="V22" s="5">
-        <f>(1/R22)*EXP(-1/R22*D22)</f>
+        <f t="shared" si="0"/>
         <v>6.2743182587734483E-4</v>
       </c>
       <c r="W22">
         <v>6.2743181000000003E-4</v>
       </c>
       <c r="X22" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>-2.5305290751731491E-8</v>
       </c>
       <c r="Z22" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0.52716757615094512</v>
       </c>
       <c r="AA22" s="7">
         <v>0.52716750000000001</v>
       </c>
       <c r="AB22" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>-1.4445301366183827E-7</v>
       </c>
     </row>
@@ -1648,47 +1689,47 @@
         <v>1</v>
       </c>
       <c r="N23">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>5.9680980999999997</v>
       </c>
       <c r="O23">
         <v>5.9680980000000003</v>
       </c>
       <c r="P23" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-1.6755756671038569E-8</v>
       </c>
       <c r="R23">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>390.7617737477799</v>
       </c>
       <c r="S23">
         <v>390.76179999999999</v>
       </c>
       <c r="T23" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>6.7182160279344316E-8</v>
       </c>
       <c r="V23" s="5">
-        <f>(1/R23)*EXP(-1/R23*D23)</f>
+        <f t="shared" si="0"/>
         <v>1.7261791355429709E-3</v>
       </c>
       <c r="W23">
         <v>1.72617915E-3</v>
       </c>
       <c r="X23" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>8.3751614532445728E-9</v>
       </c>
       <c r="Z23" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0.3254751791888193</v>
       </c>
       <c r="AA23" s="7">
         <v>0.32547520000000002</v>
       </c>
       <c r="AB23" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>6.3940914785121095E-8</v>
       </c>
     </row>
@@ -1715,47 +1756,47 @@
         <v>1</v>
       </c>
       <c r="N24">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>6.9706950999999995</v>
       </c>
       <c r="O24">
         <v>6.9706950000000001</v>
       </c>
       <c r="P24" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-1.4345771570667409E-8</v>
       </c>
       <c r="R24">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1064.9627489286352</v>
       </c>
       <c r="S24">
         <v>1064.9628</v>
       </c>
       <c r="T24" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>4.7956010496008616E-8</v>
       </c>
       <c r="V24" s="5">
-        <f>(1/R24)*EXP(-1/R24*D24)</f>
+        <f t="shared" si="0"/>
         <v>3.3792598892054131E-4</v>
       </c>
       <c r="W24">
         <v>3.3792598999999999E-4</v>
       </c>
       <c r="X24" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>3.1943641065623751E-9</v>
       </c>
       <c r="Z24" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0.64012140990475275</v>
       </c>
       <c r="AA24" s="7">
         <v>0.64012139999999995</v>
       </c>
       <c r="AB24" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>-1.5473240910779396E-8</v>
       </c>
     </row>
@@ -1782,47 +1823,47 @@
         <v>1</v>
       </c>
       <c r="N25">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>7.9732921000000001</v>
       </c>
       <c r="O25">
         <v>7.9732919999999998</v>
       </c>
       <c r="P25" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-1.2541870875182326E-8</v>
       </c>
       <c r="R25">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2902.3966334477723</v>
       </c>
       <c r="S25">
         <v>2902.3968</v>
       </c>
       <c r="T25" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>5.7384378804314906E-8</v>
       </c>
       <c r="V25" s="5">
-        <f>(1/R25)*EXP(-1/R25*D25)</f>
+        <f t="shared" si="0"/>
         <v>6.2125544626006964E-5</v>
       </c>
       <c r="W25">
         <v>6.2125550000000004E-5</v>
       </c>
       <c r="X25" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>8.6502147667033569E-8</v>
       </c>
       <c r="Z25" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0.81968702842636798</v>
       </c>
       <c r="AA25" s="7">
         <v>0.81968700000000005</v>
       </c>
       <c r="AB25" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>-3.4679538574167168E-8</v>
       </c>
       <c r="BE25" t="s">
@@ -1831,7 +1872,7 @@
     </row>
     <row r="26" spans="1:61" x14ac:dyDescent="0.3">
       <c r="AF26" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
     </row>
     <row r="27" spans="1:61" x14ac:dyDescent="0.3">
@@ -1874,7 +1915,7 @@
         <v>49</v>
       </c>
       <c r="AK28" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="AN28" t="s">
         <v>15</v>
@@ -2042,34 +2083,34 @@
         <v>-1.3143899946221893E-7</v>
       </c>
       <c r="V30">
-        <f>(R30+1)*((F30*G30)^(-(R30+1)))*((F30^(-R30)+G30^(-R30)-1)^(-(2*R30+1)/R30))</f>
+        <f t="shared" ref="V30:V39" si="8">(R30+1)*((F30*G30)^(-(R30+1)))*((F30^(-R30)+G30^(-R30)-1)^(-(2*R30+1)/R30))</f>
         <v>1.1403629596354892</v>
       </c>
       <c r="W30">
         <v>1.140363</v>
       </c>
       <c r="X30" s="1">
-        <f>W30/V30-1</f>
+        <f t="shared" ref="X30:X39" si="9">W30/V30-1</f>
         <v>3.5396195974257694E-8</v>
       </c>
       <c r="Z30">
-        <f>F30^(-R30)+G30^(-R30)-1</f>
+        <f t="shared" ref="Z30:Z39" si="10">F30^(-R30)+G30^(-R30)-1</f>
         <v>10.10237907774404</v>
       </c>
       <c r="AA30">
-        <f>1/(1+R30)</f>
+        <f t="shared" ref="AA30:AA39" si="11">1/(1+R30)</f>
         <v>0.27950423359477899</v>
       </c>
       <c r="AB30">
-        <f>-(LN(F30*G30))</f>
+        <f t="shared" ref="AB30:AB39" si="12">-(LN(F30*G30))</f>
         <v>1.2240472306089623</v>
       </c>
       <c r="AC30" s="9">
-        <f>LN(Z30)/(R30^2)</f>
+        <f t="shared" ref="AC30:AC39" si="13">LN(Z30)/(R30^2)</f>
         <v>0.34805392664123247</v>
       </c>
       <c r="AD30">
-        <f>-(2+1/R30)*((F30^(-R30))*(-LN(F30))-(G30^(-R30))*LN(G30))/(Z30)</f>
+        <f t="shared" ref="AD30:AD39" si="14">-(2+1/R30)*((F30^(-R30))*(-LN(F30))-(G30^(-R30))*LN(G30))/(Z30)</f>
         <v>-1.8718265975699773</v>
       </c>
       <c r="AE30">
@@ -2091,7 +2132,7 @@
         <v>-6.5868350000000006E-2</v>
       </c>
       <c r="AN30">
-        <f>AE30*AI30</f>
+        <f t="shared" ref="AN30:AN39" si="15">AE30*AI30</f>
         <v>-5.2125485362386537E-2</v>
       </c>
       <c r="AO30">
@@ -2164,124 +2205,124 @@
         <v>0.70469110000000001</v>
       </c>
       <c r="N31">
-        <f t="shared" ref="N31:N39" si="7">$L$11*1</f>
+        <f t="shared" ref="N31:N39" si="16">$L$11*1</f>
         <v>0.94692209999999999</v>
       </c>
       <c r="O31">
         <v>0.94692209999999999</v>
       </c>
       <c r="P31" s="1">
-        <f t="shared" ref="P31:P39" si="8">O31/N31-1</f>
+        <f t="shared" ref="P31:P39" si="17">O31/N31-1</f>
         <v>0</v>
       </c>
       <c r="R31">
-        <f t="shared" ref="R31:R39" si="9">EXP(N31)</f>
+        <f t="shared" ref="R31:R39" si="18">EXP(N31)</f>
         <v>2.5777633388186341</v>
       </c>
       <c r="S31">
         <v>2.577763</v>
       </c>
       <c r="T31" s="1">
-        <f t="shared" ref="T31:T39" si="10">S31/R31-1</f>
+        <f t="shared" ref="T31:T39" si="19">S31/R31-1</f>
         <v>-1.3143899946221893E-7</v>
       </c>
       <c r="V31">
-        <f>(R31+1)*((F31*G31)^(-(R31+1)))*((F31^(-R31)+G31^(-R31)-1)^(-(2*R31+1)/R31))</f>
+        <f t="shared" si="8"/>
         <v>1.6651163607126231</v>
       </c>
       <c r="W31">
         <v>1.6651164000000001</v>
       </c>
       <c r="X31" s="1">
-        <f>W31/V31-1</f>
+        <f t="shared" si="9"/>
         <v>2.3594373343982511E-8</v>
       </c>
       <c r="Z31">
-        <f>F31^(-R31)+G31^(-R31)-1</f>
+        <f t="shared" si="10"/>
         <v>3.9517704116616912</v>
       </c>
       <c r="AA31">
-        <f>1/(1+R31)</f>
+        <f t="shared" si="11"/>
         <v>0.27950423359477899</v>
       </c>
       <c r="AB31">
-        <f>-(LN(F31*G31))</f>
+        <f t="shared" si="12"/>
         <v>0.70339148314878785</v>
       </c>
       <c r="AC31" s="9">
-        <f>LN(Z31)/(R31^2)</f>
+        <f t="shared" si="13"/>
         <v>0.20680087943727488</v>
       </c>
       <c r="AD31">
-        <f>-(2+1/R31)*((F31^(-R31))*(-LN(F31))-(G31^(-R31))*LN(G31))/(Z31)</f>
+        <f t="shared" si="14"/>
         <v>-1.0523671414785138</v>
       </c>
       <c r="AE31">
-        <f t="shared" ref="AE31:AE39" si="11">SUM(AA31:AD31)</f>
+        <f t="shared" ref="AE31:AE39" si="20">SUM(AA31:AD31)</f>
         <v>0.13732945470232782</v>
       </c>
       <c r="AF31">
         <v>0.13732945299999999</v>
       </c>
       <c r="AG31" s="1">
-        <f t="shared" ref="AG31:AG39" si="12">AF31/AE31-1</f>
+        <f t="shared" ref="AG31:AG39" si="21">AF31/AE31-1</f>
         <v>-1.2395941162424151E-8</v>
       </c>
       <c r="AI31">
-        <f t="shared" ref="AI31:AI39" si="13">EXP(N31)</f>
+        <f t="shared" ref="AI31:AI39" si="22">EXP(N31)</f>
         <v>2.5777633388186341</v>
       </c>
       <c r="AK31">
         <v>-1.227718E-2</v>
       </c>
       <c r="AN31">
-        <f>AE31*AI31</f>
+        <f t="shared" si="15"/>
         <v>0.35400283367161495</v>
       </c>
       <c r="AO31">
-        <f t="shared" ref="AO31:AO39" si="14">AK31</f>
+        <f t="shared" ref="AO31:AO39" si="23">AK31</f>
         <v>-1.227718E-2</v>
       </c>
       <c r="AP31">
-        <f t="shared" ref="AP31:AP39" si="15">-(AO31)*AI31*AI31</f>
+        <f t="shared" ref="AP31:AP39" si="24">-(AO31)*AI31*AI31</f>
         <v>8.1580189328153474E-2</v>
       </c>
       <c r="AQ31">
-        <f t="shared" ref="AQ31:AQ39" si="16">N31+AN31/AP31</f>
+        <f t="shared" ref="AQ31:AQ39" si="25">N31+AN31/AP31</f>
         <v>5.2862456120802532</v>
       </c>
       <c r="AY31" s="6">
         <v>0.10215065</v>
       </c>
       <c r="BA31">
-        <f t="shared" ref="BA31:BA39" si="17">R31</f>
+        <f t="shared" ref="BA31:BA39" si="26">R31</f>
         <v>2.5777633388186341</v>
       </c>
       <c r="BB31">
         <v>3.310038</v>
       </c>
       <c r="BD31" s="6">
-        <f t="shared" ref="BD31:BD39" si="18">AY31*BB31</f>
+        <f t="shared" ref="BD31:BD39" si="27">AY31*BB31</f>
         <v>0.33812253322469998</v>
       </c>
       <c r="BE31">
-        <f t="shared" ref="BE31:BE39" si="19">-(AY31^2)</f>
+        <f t="shared" ref="BE31:BE39" si="28">-(AY31^2)</f>
         <v>-1.0434755295422499E-2</v>
       </c>
       <c r="BF31">
-        <f t="shared" ref="BF31:BF39" si="20">-BE31*(BB31^2)</f>
+        <f t="shared" ref="BF31:BF39" si="29">-BE31*(BB31^2)</f>
         <v>0.11432684747428835</v>
       </c>
       <c r="BG31">
-        <f t="shared" ref="BG31:BG39" si="21">BD31/BF31</f>
+        <f t="shared" ref="BG31:BG39" si="30">BD31/BF31</f>
         <v>2.9575077131444769</v>
       </c>
       <c r="BH31">
-        <f t="shared" ref="BH31:BH39" si="22">N31+BG31</f>
+        <f t="shared" ref="BH31:BH39" si="31">N31+BG31</f>
         <v>3.904429813144477</v>
       </c>
       <c r="BI31">
-        <f t="shared" ref="BI31:BI39" si="23">0.5*N31+0.5*(N31+BH31)</f>
+        <f t="shared" ref="BI31:BI39" si="32">0.5*N31+0.5*(N31+BH31)</f>
         <v>2.8991370065722384</v>
       </c>
     </row>
@@ -2308,124 +2349,124 @@
         <v>0.87627319999999997</v>
       </c>
       <c r="N32">
-        <f t="shared" si="7"/>
+        <f t="shared" si="16"/>
         <v>0.94692209999999999</v>
       </c>
       <c r="O32">
         <v>0.94692209999999999</v>
       </c>
       <c r="P32" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="R32">
-        <f t="shared" si="9"/>
+        <f t="shared" si="18"/>
         <v>2.5777633388186341</v>
       </c>
       <c r="S32">
         <v>2.577763</v>
       </c>
       <c r="T32" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="19"/>
         <v>-1.3143899946221893E-7</v>
       </c>
       <c r="V32">
-        <f>(R32+1)*((F32*G32)^(-(R32+1)))*((F32^(-R32)+G32^(-R32)-1)^(-(2*R32+1)/R32))</f>
+        <f t="shared" si="8"/>
         <v>2.1768255386708519</v>
       </c>
       <c r="W32">
         <v>2.1768257000000002</v>
       </c>
       <c r="X32" s="1">
-        <f>W32/V32-1</f>
+        <f t="shared" si="9"/>
         <v>7.4112116665858707E-8</v>
       </c>
       <c r="Z32">
-        <f>F32^(-R32)+G32^(-R32)-1</f>
+        <f t="shared" si="10"/>
         <v>1.8825660034781526</v>
       </c>
       <c r="AA32">
-        <f>1/(1+R32)</f>
+        <f t="shared" si="11"/>
         <v>0.27950423359477899</v>
       </c>
       <c r="AB32">
-        <f>-(LN(F32*G32))</f>
+        <f t="shared" si="12"/>
         <v>0.28336745640140271</v>
       </c>
       <c r="AC32" s="9">
-        <f>LN(Z32)/(R32^2)</f>
+        <f t="shared" si="13"/>
         <v>9.5206727749407916E-2</v>
       </c>
       <c r="AD32">
-        <f>-(2+1/R32)*((F32^(-R32))*(-LN(F32))-(G32^(-R32))*LN(G32))/(Z32)</f>
+        <f t="shared" si="14"/>
         <v>-0.51891903764940839</v>
       </c>
       <c r="AE32">
-        <f t="shared" si="11"/>
+        <f t="shared" si="20"/>
         <v>0.13915938009618123</v>
       </c>
       <c r="AF32">
         <v>0.139159387</v>
       </c>
       <c r="AG32" s="1">
-        <f t="shared" si="12"/>
+        <f t="shared" si="21"/>
         <v>4.9610876073913346E-8</v>
       </c>
       <c r="AI32">
-        <f t="shared" si="13"/>
+        <f t="shared" si="22"/>
         <v>2.5777633388186341</v>
       </c>
       <c r="AK32">
         <v>-4.7801059999999999E-2</v>
       </c>
       <c r="AN32">
-        <f>AE32*AI32</f>
+        <f t="shared" si="15"/>
         <v>0.35871994826466347</v>
       </c>
       <c r="AO32">
-        <f t="shared" si="14"/>
+        <f t="shared" si="23"/>
         <v>-4.7801059999999999E-2</v>
       </c>
       <c r="AP32">
-        <f t="shared" si="15"/>
+        <f t="shared" si="24"/>
         <v>0.31763153467542415</v>
       </c>
       <c r="AQ32">
-        <f t="shared" si="16"/>
+        <f t="shared" si="25"/>
         <v>2.0762808352125663</v>
       </c>
       <c r="AY32" s="6">
         <v>0.10952967</v>
       </c>
       <c r="BA32">
-        <f t="shared" si="17"/>
+        <f t="shared" si="26"/>
         <v>2.5777633388186341</v>
       </c>
       <c r="BB32">
         <v>3.310038</v>
       </c>
       <c r="BD32" s="6">
-        <f t="shared" si="18"/>
+        <f t="shared" si="27"/>
         <v>0.36254736982746</v>
       </c>
       <c r="BE32">
-        <f t="shared" si="19"/>
+        <f t="shared" si="28"/>
         <v>-1.1996748610308899E-2</v>
       </c>
       <c r="BF32">
-        <f t="shared" si="20"/>
+        <f t="shared" si="29"/>
         <v>0.13144059536880903</v>
       </c>
       <c r="BG32">
-        <f t="shared" si="21"/>
+        <f t="shared" si="30"/>
         <v>2.7582602529316662</v>
       </c>
       <c r="BH32">
-        <f t="shared" si="22"/>
+        <f t="shared" si="31"/>
         <v>3.7051823529316663</v>
       </c>
       <c r="BI32">
-        <f t="shared" si="23"/>
+        <f t="shared" si="32"/>
         <v>2.799513276465833</v>
       </c>
     </row>
@@ -2452,124 +2493,124 @@
         <v>0.33129249999999999</v>
       </c>
       <c r="N33">
-        <f t="shared" si="7"/>
+        <f t="shared" si="16"/>
         <v>0.94692209999999999</v>
       </c>
       <c r="O33">
         <v>0.94692209999999999</v>
       </c>
       <c r="P33" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="R33">
-        <f t="shared" si="9"/>
+        <f t="shared" si="18"/>
         <v>2.5777633388186341</v>
       </c>
       <c r="S33">
         <v>2.577763</v>
       </c>
       <c r="T33" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="19"/>
         <v>-1.3143899946221893E-7</v>
       </c>
       <c r="V33">
-        <f>(R33+1)*((F33*G33)^(-(R33+1)))*((F33^(-R33)+G33^(-R33)-1)^(-(2*R33+1)/R33))</f>
+        <f t="shared" si="8"/>
         <v>2.1463547168734998</v>
       </c>
       <c r="W33">
         <v>2.1463548000000001</v>
       </c>
       <c r="X33" s="1">
-        <f>W33/V33-1</f>
+        <f t="shared" si="9"/>
         <v>3.8729152995742311E-8</v>
       </c>
       <c r="Z33">
-        <f>F33^(-R33)+G33^(-R33)-1</f>
+        <f t="shared" si="10"/>
         <v>31.078165678567274</v>
       </c>
       <c r="AA33">
-        <f>1/(1+R33)</f>
+        <f t="shared" si="11"/>
         <v>0.27950423359477899</v>
       </c>
       <c r="AB33">
-        <f>-(LN(F33*G33))</f>
+        <f t="shared" si="12"/>
         <v>2.150835023422212</v>
       </c>
       <c r="AC33" s="9">
-        <f>LN(Z33)/(R33^2)</f>
+        <f t="shared" si="13"/>
         <v>0.51716718232757031</v>
       </c>
       <c r="AD33">
-        <f>-(2+1/R33)*((F33^(-R33))*(-LN(F33))-(G33^(-R33))*LN(G33))/(Z33)</f>
+        <f t="shared" si="14"/>
         <v>-2.6561139021353108</v>
       </c>
       <c r="AE33">
-        <f t="shared" si="11"/>
+        <f t="shared" si="20"/>
         <v>0.29139253720925051</v>
       </c>
       <c r="AF33">
         <v>0.29139253999999998</v>
       </c>
       <c r="AG33" s="1">
-        <f t="shared" si="12"/>
+        <f t="shared" si="21"/>
         <v>9.577285409179126E-9</v>
       </c>
       <c r="AI33">
-        <f t="shared" si="13"/>
+        <f t="shared" si="22"/>
         <v>2.5777633388186341</v>
       </c>
       <c r="AK33">
         <v>-5.4597060000000003E-2</v>
       </c>
       <c r="AN33">
-        <f>AE33*AI33</f>
+        <f t="shared" si="15"/>
         <v>0.75114099962335068</v>
       </c>
       <c r="AO33">
-        <f t="shared" si="14"/>
+        <f t="shared" si="23"/>
         <v>-5.4597060000000003E-2</v>
       </c>
       <c r="AP33">
-        <f t="shared" si="15"/>
+        <f t="shared" si="24"/>
         <v>0.36279002927061066</v>
       </c>
       <c r="AQ33">
-        <f t="shared" si="16"/>
+        <f t="shared" si="25"/>
         <v>3.0173786699711198</v>
       </c>
       <c r="AY33" s="6">
         <v>0.19133695000000001</v>
       </c>
       <c r="BA33">
-        <f t="shared" si="17"/>
+        <f t="shared" si="26"/>
         <v>2.5777633388186341</v>
       </c>
       <c r="BB33">
         <v>3.310038</v>
       </c>
       <c r="BD33" s="6">
-        <f t="shared" si="18"/>
+        <f t="shared" si="27"/>
         <v>0.63333257530410003</v>
       </c>
       <c r="BE33">
-        <f t="shared" si="19"/>
+        <f t="shared" si="28"/>
         <v>-3.6609828435302499E-2</v>
       </c>
       <c r="BF33">
-        <f t="shared" si="20"/>
+        <f t="shared" si="29"/>
         <v>0.40111015094132352</v>
       </c>
       <c r="BG33">
-        <f t="shared" si="21"/>
+        <f t="shared" si="30"/>
         <v>1.578949258246888</v>
       </c>
       <c r="BH33">
-        <f t="shared" si="22"/>
+        <f t="shared" si="31"/>
         <v>2.5258713582468881</v>
       </c>
       <c r="BI33">
-        <f t="shared" si="23"/>
+        <f t="shared" si="32"/>
         <v>2.2098577791234439</v>
       </c>
     </row>
@@ -2596,124 +2637,124 @@
         <v>0.64012139999999995</v>
       </c>
       <c r="N34">
-        <f t="shared" si="7"/>
+        <f t="shared" si="16"/>
         <v>0.94692209999999999</v>
       </c>
       <c r="O34">
         <v>0.94692209999999999</v>
       </c>
       <c r="P34" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="R34">
-        <f t="shared" si="9"/>
+        <f t="shared" si="18"/>
         <v>2.5777633388186341</v>
       </c>
       <c r="S34">
         <v>2.577763</v>
       </c>
       <c r="T34" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="19"/>
         <v>-1.3143899946221893E-7</v>
       </c>
       <c r="V34">
-        <f>(R34+1)*((F34*G34)^(-(R34+1)))*((F34^(-R34)+G34^(-R34)-1)^(-(2*R34+1)/R34))</f>
+        <f t="shared" si="8"/>
         <v>0.74655590494181556</v>
       </c>
       <c r="W34">
         <v>0.74655579999999999</v>
       </c>
       <c r="X34" s="1">
-        <f>W34/V34-1</f>
+        <f t="shared" si="9"/>
         <v>-1.405679265209514E-7</v>
       </c>
       <c r="Z34">
-        <f>F34^(-R34)+G34^(-R34)-1</f>
+        <f t="shared" si="10"/>
         <v>20.213647857487413</v>
       </c>
       <c r="AA34">
-        <f>1/(1+R34)</f>
+        <f t="shared" si="11"/>
         <v>0.27950423359477899</v>
       </c>
       <c r="AB34">
-        <f>-(LN(F34*G34))</f>
+        <f t="shared" si="12"/>
         <v>1.568566443829164</v>
       </c>
       <c r="AC34" s="9">
-        <f>LN(Z34)/(R34^2)</f>
+        <f t="shared" si="13"/>
         <v>0.45243335142109131</v>
       </c>
       <c r="AD34">
-        <f>-(2+1/R34)*((F34^(-R34))*(-LN(F34))-(G34^(-R34))*LN(G34))/(Z34)</f>
+        <f t="shared" si="14"/>
         <v>-2.560651378049859</v>
       </c>
       <c r="AE34">
-        <f t="shared" si="11"/>
+        <f t="shared" si="20"/>
         <v>-0.26014734920482452</v>
       </c>
       <c r="AF34">
         <v>-0.26014743899999998</v>
       </c>
       <c r="AG34" s="1">
-        <f t="shared" si="12"/>
+        <f t="shared" si="21"/>
         <v>3.4517044178450362E-7</v>
       </c>
       <c r="AI34">
-        <f t="shared" si="13"/>
+        <f t="shared" si="22"/>
         <v>2.5777633388186341</v>
       </c>
       <c r="AK34">
         <v>-0.12222094999999999</v>
       </c>
       <c r="AN34">
-        <f>AE34*AI34</f>
+        <f t="shared" si="15"/>
         <v>-0.67059829947104554</v>
       </c>
       <c r="AO34">
-        <f t="shared" si="14"/>
+        <f t="shared" si="23"/>
         <v>-0.12222094999999999</v>
       </c>
       <c r="AP34">
-        <f t="shared" si="15"/>
+        <f t="shared" si="24"/>
         <v>0.81214157004025178</v>
       </c>
       <c r="AQ34">
-        <f t="shared" si="16"/>
+        <f t="shared" si="25"/>
         <v>0.12120608667265731</v>
       </c>
       <c r="AY34" s="6">
         <v>-0.26542315</v>
       </c>
       <c r="BA34">
-        <f t="shared" si="17"/>
+        <f t="shared" si="26"/>
         <v>2.5777633388186341</v>
       </c>
       <c r="BB34">
         <v>3.310038</v>
       </c>
       <c r="BD34" s="6">
-        <f t="shared" si="18"/>
+        <f t="shared" si="27"/>
         <v>-0.87856071257970003</v>
       </c>
       <c r="BE34">
-        <f t="shared" si="19"/>
+        <f t="shared" si="28"/>
         <v>-7.04494485559225E-2</v>
       </c>
       <c r="BF34">
-        <f t="shared" si="20"/>
+        <f t="shared" si="29"/>
         <v>0.77186892568855026</v>
       </c>
       <c r="BG34">
-        <f t="shared" si="21"/>
+        <f t="shared" si="30"/>
         <v>-1.1382252651199487</v>
       </c>
       <c r="BH34">
-        <f t="shared" si="22"/>
+        <f t="shared" si="31"/>
         <v>-0.19130316511994871</v>
       </c>
       <c r="BI34">
-        <f t="shared" si="23"/>
+        <f t="shared" si="32"/>
         <v>0.85127051744002569</v>
       </c>
     </row>
@@ -2740,124 +2781,124 @@
         <v>0.42446489999999998</v>
       </c>
       <c r="N35">
-        <f t="shared" si="7"/>
+        <f t="shared" si="16"/>
         <v>0.94692209999999999</v>
       </c>
       <c r="O35">
         <v>0.94692209999999999</v>
       </c>
       <c r="P35" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="R35">
-        <f t="shared" si="9"/>
+        <f t="shared" si="18"/>
         <v>2.5777633388186341</v>
       </c>
       <c r="S35">
         <v>2.577763</v>
       </c>
       <c r="T35" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="19"/>
         <v>-1.3143899946221893E-7</v>
       </c>
       <c r="V35">
-        <f>(R35+1)*((F35*G35)^(-(R35+1)))*((F35^(-R35)+G35^(-R35)-1)^(-(2*R35+1)/R35))</f>
+        <f t="shared" si="8"/>
         <v>1.07766639180056</v>
       </c>
       <c r="W35">
         <v>1.0776661999999999</v>
       </c>
       <c r="X35" s="1">
-        <f>W35/V35-1</f>
+        <f t="shared" si="9"/>
         <v>-1.7797767615235216E-7</v>
       </c>
       <c r="Z35">
-        <f>F35^(-R35)+G35^(-R35)-1</f>
+        <f t="shared" si="10"/>
         <v>10.945251593182013</v>
       </c>
       <c r="AA35">
-        <f>1/(1+R35)</f>
+        <f t="shared" si="11"/>
         <v>0.27950423359477899</v>
       </c>
       <c r="AB35">
-        <f>-(LN(F35*G35))</f>
+        <f t="shared" si="12"/>
         <v>1.2617265910851021</v>
       </c>
       <c r="AC35" s="9">
-        <f>LN(Z35)/(R35^2)</f>
+        <f t="shared" si="13"/>
         <v>0.36011358225357754</v>
       </c>
       <c r="AD35">
-        <f>-(2+1/R35)*((F35^(-R35))*(-LN(F35))-(G35^(-R35))*LN(G35))/(Z35)</f>
+        <f t="shared" si="14"/>
         <v>-1.9531897800143319</v>
       </c>
       <c r="AE35">
-        <f t="shared" si="11"/>
+        <f t="shared" si="20"/>
         <v>-5.1845373080873225E-2</v>
       </c>
       <c r="AF35">
         <v>-5.1845467999999999E-2</v>
       </c>
       <c r="AG35" s="1">
-        <f t="shared" si="12"/>
+        <f t="shared" si="21"/>
         <v>1.8308119149601509E-6</v>
       </c>
       <c r="AI35">
-        <f t="shared" si="13"/>
+        <f t="shared" si="22"/>
         <v>2.5777633388186341</v>
       </c>
       <c r="AK35">
         <v>-7.411529E-2</v>
       </c>
       <c r="AN35">
-        <f>AE35*AI35</f>
+        <f t="shared" si="15"/>
         <v>-0.13364510201524948</v>
       </c>
       <c r="AO35">
-        <f t="shared" si="14"/>
+        <f t="shared" si="23"/>
         <v>-7.411529E-2</v>
       </c>
       <c r="AP35">
-        <f t="shared" si="15"/>
+        <f t="shared" si="24"/>
         <v>0.49248600984191809</v>
       </c>
       <c r="AQ35">
-        <f t="shared" si="16"/>
+        <f t="shared" si="25"/>
         <v>0.67555377817061868</v>
       </c>
       <c r="AY35" s="6">
         <v>-0.20778311999999999</v>
       </c>
       <c r="BA35">
-        <f t="shared" si="17"/>
+        <f t="shared" si="26"/>
         <v>2.5777633388186341</v>
       </c>
       <c r="BB35">
         <v>3.310038</v>
       </c>
       <c r="BD35" s="6">
-        <f t="shared" si="18"/>
+        <f t="shared" si="27"/>
         <v>-0.68777002295855993</v>
       </c>
       <c r="BE35">
-        <f t="shared" si="19"/>
+        <f t="shared" si="28"/>
         <v>-4.3173824956934392E-2</v>
       </c>
       <c r="BF35">
-        <f t="shared" si="20"/>
+        <f t="shared" si="29"/>
         <v>0.47302760448041808</v>
       </c>
       <c r="BG35">
-        <f t="shared" si="21"/>
+        <f t="shared" si="30"/>
         <v>-1.4539743905940092</v>
       </c>
       <c r="BH35">
-        <f t="shared" si="22"/>
+        <f t="shared" si="31"/>
         <v>-0.50705229059400925</v>
       </c>
       <c r="BI35">
-        <f t="shared" si="23"/>
+        <f t="shared" si="32"/>
         <v>0.69339595470299531</v>
       </c>
     </row>
@@ -2884,124 +2925,124 @@
         <v>0.35559689999999999</v>
       </c>
       <c r="N36">
-        <f t="shared" si="7"/>
+        <f t="shared" si="16"/>
         <v>0.94692209999999999</v>
       </c>
       <c r="O36">
         <v>0.94692209999999999</v>
       </c>
       <c r="P36" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="R36">
-        <f t="shared" si="9"/>
+        <f t="shared" si="18"/>
         <v>2.5777633388186341</v>
       </c>
       <c r="S36">
         <v>2.577763</v>
       </c>
       <c r="T36" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="19"/>
         <v>-1.3143899946221893E-7</v>
       </c>
       <c r="V36">
-        <f>(R36+1)*((F36*G36)^(-(R36+1)))*((F36^(-R36)+G36^(-R36)-1)^(-(2*R36+1)/R36))</f>
+        <f t="shared" si="8"/>
         <v>0.69063101077496047</v>
       </c>
       <c r="W36">
         <v>0.69063110000000005</v>
       </c>
       <c r="X36" s="1">
-        <f>W36/V36-1</f>
+        <f t="shared" si="9"/>
         <v>1.2919350300677479E-7</v>
       </c>
       <c r="Z36">
-        <f>F36^(-R36)+G36^(-R36)-1</f>
+        <f t="shared" si="10"/>
         <v>15.837263172599798</v>
       </c>
       <c r="AA36">
-        <f>1/(1+R36)</f>
+        <f t="shared" si="11"/>
         <v>0.27950423359477899</v>
       </c>
       <c r="AB36">
-        <f>-(LN(F36*G36))</f>
+        <f t="shared" si="12"/>
         <v>1.3839532212573171</v>
       </c>
       <c r="AC36" s="9">
-        <f>LN(Z36)/(R36^2)</f>
+        <f t="shared" si="13"/>
         <v>0.41571440171296797</v>
       </c>
       <c r="AD36">
-        <f>-(2+1/R36)*((F36^(-R36))*(-LN(F36))-(G36^(-R36))*LN(G36))/(Z36)</f>
+        <f t="shared" si="14"/>
         <v>-2.3707083641453206</v>
       </c>
       <c r="AE36">
-        <f t="shared" si="11"/>
+        <f t="shared" si="20"/>
         <v>-0.29153650758025629</v>
       </c>
       <c r="AF36">
         <v>-0.29153642299999999</v>
       </c>
       <c r="AG36" s="1">
-        <f t="shared" si="12"/>
+        <f t="shared" si="21"/>
         <v>-2.9011891855557081E-7</v>
       </c>
       <c r="AI36">
-        <f t="shared" si="13"/>
+        <f t="shared" si="22"/>
         <v>2.5777633388186341</v>
       </c>
       <c r="AK36">
         <v>-0.11047878</v>
       </c>
       <c r="AN36">
-        <f>AE36*AI36</f>
+        <f t="shared" si="15"/>
         <v>-0.75151212116760546</v>
       </c>
       <c r="AO36">
-        <f t="shared" si="14"/>
+        <f t="shared" si="23"/>
         <v>-0.11047878</v>
       </c>
       <c r="AP36">
-        <f t="shared" si="15"/>
+        <f t="shared" si="24"/>
         <v>0.73411644931029896</v>
       </c>
       <c r="AQ36">
-        <f t="shared" si="16"/>
+        <f t="shared" si="25"/>
         <v>-7.6773966031008833E-2</v>
       </c>
       <c r="AY36" s="6">
         <v>-1.0873610000000001E-2</v>
       </c>
       <c r="BA36">
-        <f t="shared" si="17"/>
+        <f t="shared" si="26"/>
         <v>2.5777633388186341</v>
       </c>
       <c r="BB36">
         <v>3.310038</v>
       </c>
       <c r="BD36" s="6">
-        <f t="shared" si="18"/>
+        <f t="shared" si="27"/>
         <v>-3.5992062297180001E-2</v>
       </c>
       <c r="BE36">
-        <f t="shared" si="19"/>
+        <f t="shared" si="28"/>
         <v>-1.1823539443210001E-4</v>
       </c>
       <c r="BF36">
-        <f t="shared" si="20"/>
+        <f t="shared" si="29"/>
         <v>1.2954285484040862E-3</v>
       </c>
       <c r="BG36">
-        <f t="shared" si="21"/>
+        <f t="shared" si="30"/>
         <v>-27.783903899231429</v>
       </c>
       <c r="BH36">
-        <f t="shared" si="22"/>
+        <f t="shared" si="31"/>
         <v>-26.836981799231431</v>
       </c>
       <c r="BI36">
-        <f t="shared" si="23"/>
+        <f t="shared" si="32"/>
         <v>-12.471568799615717</v>
       </c>
     </row>
@@ -3028,124 +3069,124 @@
         <v>0.67684909999999998</v>
       </c>
       <c r="N37">
-        <f t="shared" si="7"/>
+        <f t="shared" si="16"/>
         <v>0.94692209999999999</v>
       </c>
       <c r="O37">
         <v>0.94692209999999999</v>
       </c>
       <c r="P37" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="R37">
-        <f t="shared" si="9"/>
+        <f t="shared" si="18"/>
         <v>2.5777633388186341</v>
       </c>
       <c r="S37">
         <v>2.577763</v>
       </c>
       <c r="T37" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="19"/>
         <v>-1.3143899946221893E-7</v>
       </c>
       <c r="V37">
-        <f>(R37+1)*((F37*G37)^(-(R37+1)))*((F37^(-R37)+G37^(-R37)-1)^(-(2*R37+1)/R37))</f>
+        <f t="shared" si="8"/>
         <v>1.5082461834713472</v>
       </c>
       <c r="W37">
         <v>1.5082461</v>
       </c>
       <c r="X37" s="1">
-        <f>W37/V37-1</f>
+        <f t="shared" si="9"/>
         <v>-5.534331737333531E-8</v>
       </c>
       <c r="Z37">
-        <f>F37^(-R37)+G37^(-R37)-1</f>
+        <f t="shared" si="10"/>
         <v>3.1405655750945147</v>
       </c>
       <c r="AA37">
-        <f>1/(1+R37)</f>
+        <f t="shared" si="11"/>
         <v>0.27950423359477899</v>
       </c>
       <c r="AB37">
-        <f>-(LN(F37*G37))</f>
+        <f t="shared" si="12"/>
         <v>0.5223842905618622</v>
       </c>
       <c r="AC37" s="9">
-        <f>LN(Z37)/(R37^2)</f>
+        <f t="shared" si="13"/>
         <v>0.17222368016419781</v>
       </c>
       <c r="AD37">
-        <f>-(2+1/R37)*((F37^(-R37))*(-LN(F37))-(G37^(-R37))*LN(G37))/(Z37)</f>
+        <f t="shared" si="14"/>
         <v>-0.95281447947645614</v>
       </c>
       <c r="AE37">
-        <f t="shared" si="11"/>
+        <f t="shared" si="20"/>
         <v>2.1297724844382859E-2</v>
       </c>
       <c r="AF37">
         <v>2.1297704000000001E-2</v>
       </c>
       <c r="AG37" s="1">
-        <f t="shared" si="12"/>
+        <f t="shared" si="21"/>
         <v>-9.7871406501415237E-7</v>
       </c>
       <c r="AI37">
-        <f t="shared" si="13"/>
+        <f t="shared" si="22"/>
         <v>2.5777633388186341</v>
       </c>
       <c r="AK37">
         <v>-4.6903170000000001E-2</v>
       </c>
       <c r="AN37">
-        <f>AE37*AI37</f>
+        <f t="shared" si="15"/>
         <v>5.4900494304096936E-2</v>
       </c>
       <c r="AO37">
-        <f t="shared" si="14"/>
+        <f t="shared" si="23"/>
         <v>-4.6903170000000001E-2</v>
       </c>
       <c r="AP37">
-        <f t="shared" si="15"/>
+        <f t="shared" si="24"/>
         <v>0.31166517789024584</v>
       </c>
       <c r="AQ37">
-        <f t="shared" si="16"/>
+        <f t="shared" si="25"/>
         <v>1.1230742600704149</v>
       </c>
       <c r="AY37" s="6">
         <v>1.0813379999999999E-2</v>
       </c>
       <c r="BA37">
-        <f t="shared" si="17"/>
+        <f t="shared" si="26"/>
         <v>2.5777633388186341</v>
       </c>
       <c r="BB37">
         <v>3.310038</v>
       </c>
       <c r="BD37" s="6">
-        <f t="shared" si="18"/>
+        <f t="shared" si="27"/>
         <v>3.5792698708439999E-2</v>
       </c>
       <c r="BE37">
-        <f t="shared" si="19"/>
+        <f t="shared" si="28"/>
         <v>-1.1692918702439999E-4</v>
       </c>
       <c r="BF37">
-        <f t="shared" si="20"/>
+        <f t="shared" si="29"/>
         <v>1.2811172808331623E-3</v>
       </c>
       <c r="BG37">
-        <f t="shared" si="21"/>
+        <f t="shared" si="30"/>
         <v>27.938658890903852</v>
       </c>
       <c r="BH37">
-        <f t="shared" si="22"/>
+        <f t="shared" si="31"/>
         <v>28.885580990903851</v>
       </c>
       <c r="BI37">
-        <f t="shared" si="23"/>
+        <f t="shared" si="32"/>
         <v>15.389712595451924</v>
       </c>
     </row>
@@ -3172,124 +3213,124 @@
         <v>0.52716750000000001</v>
       </c>
       <c r="N38">
-        <f t="shared" si="7"/>
+        <f t="shared" si="16"/>
         <v>0.94692209999999999</v>
       </c>
       <c r="O38">
         <v>0.94692209999999999</v>
       </c>
       <c r="P38" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="R38">
-        <f t="shared" si="9"/>
+        <f t="shared" si="18"/>
         <v>2.5777633388186341</v>
       </c>
       <c r="S38">
         <v>2.577763</v>
       </c>
       <c r="T38" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="19"/>
         <v>-1.3143899946221893E-7</v>
       </c>
       <c r="V38">
-        <f>(R38+1)*((F38*G38)^(-(R38+1)))*((F38^(-R38)+G38^(-R38)-1)^(-(2*R38+1)/R38))</f>
+        <f t="shared" si="8"/>
         <v>1.2167637935291888</v>
       </c>
       <c r="W38">
         <v>1.2167635000000001</v>
       </c>
       <c r="X38" s="1">
-        <f>W38/V38-1</f>
+        <f t="shared" si="9"/>
         <v>-2.4123760933303373E-7</v>
       </c>
       <c r="Z38">
-        <f>F38^(-R38)+G38^(-R38)-1</f>
+        <f t="shared" si="10"/>
         <v>21.458631129299981</v>
       </c>
       <c r="AA38">
-        <f>1/(1+R38)</f>
+        <f t="shared" si="11"/>
         <v>0.27950423359477899</v>
       </c>
       <c r="AB38">
-        <f>-(LN(F38*G38))</f>
+        <f t="shared" si="12"/>
         <v>1.7449905521529459</v>
       </c>
       <c r="AC38" s="9">
-        <f>LN(Z38)/(R38^2)</f>
+        <f t="shared" si="13"/>
         <v>0.46142810839932841</v>
       </c>
       <c r="AD38">
-        <f>-(2+1/R38)*((F38^(-R38))*(-LN(F38))-(G38^(-R38))*LN(G38))/(Z38)</f>
+        <f t="shared" si="14"/>
         <v>-2.4917555144355168</v>
       </c>
       <c r="AE38">
-        <f t="shared" si="11"/>
+        <f t="shared" si="20"/>
         <v>-5.8326202884635414E-3</v>
       </c>
       <c r="AF38">
         <v>-5.832762E-3</v>
       </c>
       <c r="AG38" s="1">
-        <f t="shared" si="12"/>
+        <f t="shared" si="21"/>
         <v>2.4296376148313925E-5</v>
       </c>
       <c r="AI38">
-        <f t="shared" si="13"/>
+        <f t="shared" si="22"/>
         <v>2.5777633388186341</v>
       </c>
       <c r="AK38">
         <v>-0.1023525</v>
       </c>
       <c r="AN38">
-        <f>AE38*AI38</f>
+        <f t="shared" si="15"/>
         <v>-1.5035114748851082E-2</v>
       </c>
       <c r="AO38">
-        <f t="shared" si="14"/>
+        <f t="shared" si="23"/>
         <v>-0.1023525</v>
       </c>
       <c r="AP38">
-        <f t="shared" si="15"/>
+        <f t="shared" si="24"/>
         <v>0.68011842525806643</v>
       </c>
       <c r="AQ38">
-        <f t="shared" si="16"/>
+        <f t="shared" si="25"/>
         <v>0.92481548710659678</v>
       </c>
       <c r="AY38" s="6">
         <v>-1.3418899999999999E-2</v>
       </c>
       <c r="BA38">
-        <f t="shared" si="17"/>
+        <f t="shared" si="26"/>
         <v>2.5777633388186341</v>
       </c>
       <c r="BB38">
         <v>3.310038</v>
       </c>
       <c r="BD38" s="6">
-        <f t="shared" si="18"/>
+        <f t="shared" si="27"/>
         <v>-4.4417068918199999E-2</v>
       </c>
       <c r="BE38">
-        <f t="shared" si="19"/>
+        <f t="shared" si="28"/>
         <v>-1.8006687720999997E-4</v>
       </c>
       <c r="BF38">
-        <f t="shared" si="20"/>
+        <f t="shared" si="29"/>
         <v>1.9728760112841283E-3</v>
       </c>
       <c r="BG38">
-        <f t="shared" si="21"/>
+        <f t="shared" si="30"/>
         <v>-22.513867401778231</v>
       </c>
       <c r="BH38">
-        <f t="shared" si="22"/>
+        <f t="shared" si="31"/>
         <v>-21.566945301778233</v>
       </c>
       <c r="BI38">
-        <f t="shared" si="23"/>
+        <f t="shared" si="32"/>
         <v>-9.8365505508891182</v>
       </c>
     </row>
@@ -3316,124 +3357,124 @@
         <v>0.81968700000000005</v>
       </c>
       <c r="N39">
-        <f t="shared" si="7"/>
+        <f t="shared" si="16"/>
         <v>0.94692209999999999</v>
       </c>
       <c r="O39">
         <v>0.94692209999999999</v>
       </c>
       <c r="P39" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="R39">
-        <f t="shared" si="9"/>
+        <f t="shared" si="18"/>
         <v>2.5777633388186341</v>
       </c>
       <c r="S39">
         <v>2.577763</v>
       </c>
       <c r="T39" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="19"/>
         <v>-1.3143899946221893E-7</v>
       </c>
       <c r="V39">
-        <f>(R39+1)*((F39*G39)^(-(R39+1)))*((F39^(-R39)+G39^(-R39)-1)^(-(2*R39+1)/R39))</f>
+        <f t="shared" si="8"/>
         <v>1.4579381052359415</v>
       </c>
       <c r="W39">
         <v>1.4579381</v>
       </c>
       <c r="X39" s="1">
-        <f>W39/V39-1</f>
+        <f t="shared" si="9"/>
         <v>-3.5913331197789944E-9</v>
       </c>
       <c r="Z39">
-        <f>F39^(-R39)+G39^(-R39)-1</f>
+        <f t="shared" si="10"/>
         <v>3.8275158171018226</v>
       </c>
       <c r="AA39">
-        <f>1/(1+R39)</f>
+        <f t="shared" si="11"/>
         <v>0.27950423359477899</v>
       </c>
       <c r="AB39">
-        <f>-(LN(F39*G39))</f>
+        <f t="shared" si="12"/>
         <v>0.64493015202651161</v>
       </c>
       <c r="AC39" s="9">
-        <f>LN(Z39)/(R39^2)</f>
+        <f t="shared" si="13"/>
         <v>0.20199300018414709</v>
       </c>
       <c r="AD39">
-        <f>-(2+1/R39)*((F39^(-R39))*(-LN(F39))-(G39^(-R39))*LN(G39))/(Z39)</f>
+        <f t="shared" si="14"/>
         <v>-1.0860143824602919</v>
       </c>
       <c r="AE39">
-        <f t="shared" si="11"/>
+        <f t="shared" si="20"/>
         <v>4.0413003345145748E-2</v>
       </c>
       <c r="AF39">
         <v>4.0412992000000002E-2</v>
       </c>
       <c r="AG39" s="1">
-        <f t="shared" si="12"/>
+        <f t="shared" si="21"/>
         <v>-2.8073008206952466E-7</v>
       </c>
       <c r="AI39">
-        <f t="shared" si="13"/>
+        <f t="shared" si="22"/>
         <v>2.5777633388186341</v>
       </c>
       <c r="AK39">
         <v>-3.7304209999999997E-2</v>
       </c>
       <c r="AN39">
-        <f>AE39*AI39</f>
+        <f t="shared" si="15"/>
         <v>0.10417515843467152</v>
       </c>
       <c r="AO39">
-        <f t="shared" si="14"/>
+        <f t="shared" si="23"/>
         <v>-3.7304209999999997E-2</v>
       </c>
       <c r="AP39">
-        <f t="shared" si="15"/>
+        <f t="shared" si="24"/>
         <v>0.24788139577143903</v>
       </c>
       <c r="AQ39">
-        <f t="shared" si="16"/>
+        <f t="shared" si="25"/>
         <v>1.3671842100727021</v>
       </c>
       <c r="AY39" s="6">
         <v>7.7398289999999995E-2</v>
       </c>
       <c r="BA39">
-        <f t="shared" si="17"/>
+        <f t="shared" si="26"/>
         <v>2.5777633388186341</v>
       </c>
       <c r="BB39">
         <v>3.310038</v>
       </c>
       <c r="BD39" s="6">
-        <f t="shared" si="18"/>
+        <f t="shared" si="27"/>
         <v>0.25619128103501998</v>
       </c>
       <c r="BE39">
-        <f t="shared" si="19"/>
+        <f t="shared" si="28"/>
         <v>-5.9904952949240992E-3</v>
       </c>
       <c r="BF39">
-        <f t="shared" si="20"/>
+        <f t="shared" si="29"/>
         <v>6.5633972478364597E-2</v>
       </c>
       <c r="BG39">
-        <f t="shared" si="21"/>
+        <f t="shared" si="30"/>
         <v>3.9033334622473168</v>
       </c>
       <c r="BH39">
-        <f t="shared" si="22"/>
+        <f t="shared" si="31"/>
         <v>4.8502555622473169</v>
       </c>
       <c r="BI39">
-        <f t="shared" si="23"/>
+        <f t="shared" si="32"/>
         <v>3.3720498811236586</v>
       </c>
     </row>
@@ -3451,19 +3492,19 @@
         <v>-6.3118717417440014E-3</v>
       </c>
       <c r="BE40" s="6">
-        <f t="shared" ref="BE40:BH40" si="24">AVERAGE(BE30:BE39)</f>
+        <f t="shared" ref="BE40:BH40" si="33">AVERAGE(BE30:BE39)</f>
         <v>-1.7923414803240299E-2</v>
       </c>
       <c r="BF40" s="6">
-        <f t="shared" si="24"/>
+        <f t="shared" si="33"/>
         <v>0.19637523376589033</v>
       </c>
       <c r="BG40" s="6">
-        <f t="shared" si="24"/>
+        <f t="shared" si="33"/>
         <v>-3.7357479764200305</v>
       </c>
       <c r="BH40" s="6">
-        <f t="shared" si="24"/>
+        <f t="shared" si="33"/>
         <v>-2.7888258764200313</v>
       </c>
       <c r="BI40" s="6">
@@ -3473,7 +3514,7 @@
     </row>
     <row r="41" spans="1:61" x14ac:dyDescent="0.3">
       <c r="V41" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="AP41">
         <f>AVERAGE(N30:N39)</f>
@@ -3492,7 +3533,7 @@
     </row>
     <row r="43" spans="1:61" x14ac:dyDescent="0.3">
       <c r="V43">
-        <f t="shared" ref="V43:V51" si="25">LN(V31)</f>
+        <f t="shared" ref="V43:V51" si="34">LN(V31)</f>
         <v>0.50989500730436021</v>
       </c>
       <c r="AP43">
@@ -3502,7 +3543,7 @@
     </row>
     <row r="44" spans="1:61" x14ac:dyDescent="0.3">
       <c r="V44">
-        <f t="shared" si="25"/>
+        <f t="shared" si="34"/>
         <v>0.7778676406262971</v>
       </c>
       <c r="AP44">
@@ -3512,7 +3553,7 @@
     </row>
     <row r="45" spans="1:61" x14ac:dyDescent="0.3">
       <c r="V45">
-        <f t="shared" si="25"/>
+        <f t="shared" si="34"/>
         <v>0.76377092266180546</v>
       </c>
       <c r="AG45" t="s">
@@ -3521,14 +3562,14 @@
     </row>
     <row r="46" spans="1:61" x14ac:dyDescent="0.3">
       <c r="V46">
-        <f t="shared" si="25"/>
+        <f t="shared" si="34"/>
         <v>-0.29228477540064668</v>
       </c>
       <c r="AG46" t="s">
         <v>41</v>
       </c>
       <c r="AO46" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="AP46">
         <f>L11</f>
@@ -3537,7 +3578,7 @@
     </row>
     <row r="47" spans="1:61" x14ac:dyDescent="0.3">
       <c r="V47">
-        <f t="shared" si="25"/>
+        <f t="shared" si="34"/>
         <v>7.4797955018451073E-2</v>
       </c>
       <c r="AG47" s="3" t="s">
@@ -3550,7 +3591,7 @@
         <v>27</v>
       </c>
       <c r="AO47" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="AP47">
         <f>AP44*AP43</f>
@@ -3559,59 +3600,59 @@
     </row>
     <row r="48" spans="1:61" x14ac:dyDescent="0.3">
       <c r="V48">
-        <f t="shared" si="25"/>
+        <f t="shared" si="34"/>
         <v>-0.37014959092933547</v>
       </c>
       <c r="AB48" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="AG48">
-        <f>MAX((F30^(-R30)+G30^(-R30)-1)^(-1/R30),0)</f>
+        <f t="shared" ref="AG48:AG57" si="35">MAX((F30^(-R30)+G30^(-R30)-1)^(-1/R30),0)</f>
         <v>0.40770938419160974</v>
       </c>
     </row>
     <row r="49" spans="18:33" x14ac:dyDescent="0.3">
       <c r="V49">
-        <f t="shared" si="25"/>
+        <f t="shared" si="34"/>
         <v>0.41094750790049006</v>
       </c>
       <c r="AB49" t="s">
         <v>16</v>
       </c>
       <c r="AG49">
-        <f>MAX((F31^(-R31)+G31^(-R31)-1)^(-1/R31),0)</f>
+        <f t="shared" si="35"/>
         <v>0.5867926693085701</v>
       </c>
     </row>
     <row r="50" spans="18:33" x14ac:dyDescent="0.3">
       <c r="V50">
-        <f t="shared" si="25"/>
+        <f t="shared" si="34"/>
         <v>0.19619470603798522</v>
       </c>
       <c r="AB50" t="s">
         <v>17</v>
       </c>
       <c r="AG50">
-        <f>MAX((F32^(-R32)+G32^(-R32)-1)^(-1/R32),0)</f>
+        <f t="shared" si="35"/>
         <v>0.78237554870791493</v>
       </c>
     </row>
     <row r="51" spans="18:33" x14ac:dyDescent="0.3">
       <c r="V51">
-        <f t="shared" si="25"/>
+        <f t="shared" si="34"/>
         <v>0.37702318085816144</v>
       </c>
       <c r="AB51" t="s">
         <v>18</v>
       </c>
       <c r="AG51">
-        <f>MAX((F33^(-R33)+G33^(-R33)-1)^(-1/R33),0)</f>
+        <f t="shared" si="35"/>
         <v>0.26364952816223569</v>
       </c>
     </row>
     <row r="52" spans="18:33" x14ac:dyDescent="0.3">
       <c r="U52" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="V52">
         <f>SUM(V42:V51)</f>
@@ -3621,7 +3662,7 @@
         <v>19</v>
       </c>
       <c r="AG52">
-        <f>MAX((F34^(-R34)+G34^(-R34)-1)^(-1/R34),0)</f>
+        <f t="shared" si="35"/>
         <v>0.31152798461104519</v>
       </c>
     </row>
@@ -3630,7 +3671,7 @@
         <v>20</v>
       </c>
       <c r="AG53">
-        <f>MAX((F35^(-R35)+G35^(-R35)-1)^(-1/R35),0)</f>
+        <f t="shared" si="35"/>
         <v>0.39522992684863228</v>
       </c>
     </row>
@@ -3639,7 +3680,7 @@
         <v>21</v>
       </c>
       <c r="AG54">
-        <f>MAX((F36^(-R36)+G36^(-R36)-1)^(-1/R36),0)</f>
+        <f t="shared" si="35"/>
         <v>0.34245557279707128</v>
       </c>
     </row>
@@ -3648,7 +3689,7 @@
         <v>22</v>
       </c>
       <c r="AG55">
-        <f>MAX((F37^(-R37)+G37^(-R37)-1)^(-1/R37),0)</f>
+        <f t="shared" si="35"/>
         <v>0.64149628323851182</v>
       </c>
     </row>
@@ -3657,7 +3698,7 @@
         <v>23</v>
       </c>
       <c r="AG56">
-        <f>MAX((F38^(-R38)+G38^(-R38)-1)^(-1/R38),0)</f>
+        <f t="shared" si="35"/>
         <v>0.30438788258321925</v>
       </c>
     </row>
@@ -3666,7 +3707,7 @@
         <v>24</v>
       </c>
       <c r="AG57">
-        <f>MAX((F39^(-R39)+G39^(-R39)-1)^(-1/R39),0)</f>
+        <f t="shared" si="35"/>
         <v>0.59411038082836709</v>
       </c>
     </row>
@@ -3821,6 +3862,295 @@
       </c>
       <c r="X73">
         <v>1.4579381</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2EE65FA-DA57-477E-BF5B-BFCA806169CC}">
+  <dimension ref="A2:P16"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="4" max="12" width="15.5546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A2" s="3" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="B3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D3" t="s">
+        <v>77</v>
+      </c>
+      <c r="E3" t="s">
+        <v>78</v>
+      </c>
+      <c r="F3" t="s">
+        <v>79</v>
+      </c>
+      <c r="G3" t="s">
+        <v>69</v>
+      </c>
+      <c r="H3" t="s">
+        <v>70</v>
+      </c>
+      <c r="I3" t="s">
+        <v>71</v>
+      </c>
+      <c r="J3" t="s">
+        <v>72</v>
+      </c>
+      <c r="K3" t="s">
+        <v>3</v>
+      </c>
+      <c r="L3" t="s">
+        <v>5</v>
+      </c>
+      <c r="N3" t="s">
+        <v>8</v>
+      </c>
+      <c r="O3" t="s">
+        <v>80</v>
+      </c>
+      <c r="P3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4" s="7">
+        <v>21.692740000000001</v>
+      </c>
+      <c r="E4" s="7">
+        <v>1.4982830000000001E-2</v>
+      </c>
+      <c r="F4" s="7">
+        <v>0.44076359999999998</v>
+      </c>
+      <c r="G4" s="7">
+        <v>37.325150000000001</v>
+      </c>
+      <c r="H4" s="7">
+        <v>-1.12207709E-2</v>
+      </c>
+      <c r="I4" s="7">
+        <v>-7.8213740000000007E-3</v>
+      </c>
+      <c r="J4" s="7">
+        <v>-1.6845708000000001E-2</v>
+      </c>
+      <c r="K4" s="7">
+        <v>7</v>
+      </c>
+      <c r="L4" s="7">
+        <v>0</v>
+      </c>
+      <c r="N4">
+        <v>2.61707</v>
+      </c>
+      <c r="O4" t="s">
+        <v>81</v>
+      </c>
+      <c r="P4">
+        <v>1.2878540000000001</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A5" s="3">
+        <v>2</v>
+      </c>
+      <c r="B5" s="3">
+        <v>2</v>
+      </c>
+      <c r="C5" s="3">
+        <v>1</v>
+      </c>
+      <c r="D5" s="10">
+        <v>111.89069000000001</v>
+      </c>
+      <c r="E5" s="10">
+        <v>3.2724809999999998E-3</v>
+      </c>
+      <c r="F5" s="10">
+        <v>0.66710979999999998</v>
+      </c>
+      <c r="G5" s="10">
+        <v>101.72411</v>
+      </c>
+      <c r="H5" s="10">
+        <v>9.8248749999999994E-4</v>
+      </c>
+      <c r="I5" s="10">
+        <v>-1.3008244E-2</v>
+      </c>
+      <c r="J5" s="10">
+        <v>-1.1679E-2</v>
+      </c>
+      <c r="K5" s="10">
+        <v>7</v>
+      </c>
+      <c r="L5" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>3</v>
+      </c>
+      <c r="B6">
+        <v>3</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6" s="7">
+        <v>153.15924000000001</v>
+      </c>
+      <c r="E6" s="7">
+        <v>2.0759910000000001E-3</v>
+      </c>
+      <c r="F6" s="7">
+        <v>0.42446489999999998</v>
+      </c>
+      <c r="G6" s="7">
+        <v>277.23385000000002</v>
+      </c>
+      <c r="H6" s="7">
+        <v>-1.6143228999999999E-3</v>
+      </c>
+      <c r="I6" s="7">
+        <v>5.2690109999999997E-3</v>
+      </c>
+      <c r="J6" s="7">
+        <v>5.1667079999999999E-3</v>
+      </c>
+      <c r="K6" s="7">
+        <v>7</v>
+      </c>
+      <c r="L6" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A8" s="3" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="B9" t="s">
+        <v>36</v>
+      </c>
+      <c r="C9" t="s">
+        <v>37</v>
+      </c>
+      <c r="D9" t="s">
+        <v>38</v>
+      </c>
+      <c r="E9" t="s">
+        <v>39</v>
+      </c>
+      <c r="F9" t="s">
+        <v>75</v>
+      </c>
+      <c r="G9" t="s">
+        <v>76</v>
+      </c>
+      <c r="H9" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>1</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+      <c r="D10">
+        <v>2</v>
+      </c>
+      <c r="E10">
+        <v>1</v>
+      </c>
+      <c r="F10" s="7">
+        <v>5.9091100000000001</v>
+      </c>
+      <c r="G10" s="7">
+        <v>-4.9349999999999996</v>
+      </c>
+      <c r="H10" s="7">
+        <v>1.076902</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>2</v>
+      </c>
+      <c r="B11">
+        <v>2</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
+      <c r="D11">
+        <v>3</v>
+      </c>
+      <c r="E11">
+        <v>1</v>
+      </c>
+      <c r="F11" s="7">
+        <v>-4.7496029999999996</v>
+      </c>
+      <c r="G11" s="7">
+        <v>5.8967850000000004</v>
+      </c>
+      <c r="H11" s="7">
+        <v>0.98058409999999996</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="C14" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="D15" t="s">
+        <v>84</v>
+      </c>
+      <c r="E15" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="D16" s="7">
+        <f>F11</f>
+        <v>-4.7496029999999996</v>
       </c>
     </row>
   </sheetData>

</xml_diff>